<commit_message>
More BSP tag discovery
</commit_message>
<xml_diff>
--- a/Research/BSP Layout.xlsx
+++ b/Research/BSP Layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ron\Desktop\openh2\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12ABFD8-D3E2-44CB-A2CC-6A4EBD0B2668}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2926F6-1BCD-4C34-8C5E-9B4A86B764EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="8100" xr2:uid="{7C22A468-B651-4234-BD2F-70F5ECA787F1}"/>
+    <workbookView xWindow="34035" yWindow="2310" windowWidth="21600" windowHeight="11505" xr2:uid="{7C22A468-B651-4234-BD2F-70F5ECA787F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="71">
   <si>
     <t>File size</t>
   </si>
@@ -105,9 +105,6 @@
     <t>int, offset, 28 data</t>
   </si>
   <si>
-    <t>Something with an offset and floats</t>
-  </si>
-  <si>
     <t>64x 0xFF</t>
   </si>
   <si>
@@ -238,6 +235,15 @@
   </si>
   <si>
     <t>Half edge</t>
+  </si>
+  <si>
+    <t>Last short is material index - material (I believe) is just shader / metadata</t>
+  </si>
+  <si>
+    <t>Collision data</t>
+  </si>
+  <si>
+    <t>Clusters/render chunks</t>
   </si>
 </sst>
 </file>
@@ -994,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5402844C-0554-4902-B07C-5C11243F8396}">
   <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,7 +1041,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>2</v>
@@ -1097,7 +1103,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>2</v>
@@ -1112,7 +1118,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1159,7 +1165,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1179,7 +1188,7 @@
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
       <c r="J14" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1197,7 +1206,7 @@
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
       <c r="J15" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1230,7 +1239,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1250,7 +1259,7 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1268,10 +1277,10 @@
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1322,7 +1331,7 @@
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
       <c r="J20" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1340,7 +1349,7 @@
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
       <c r="J21" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1373,7 +1382,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1393,7 +1402,7 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1411,7 +1420,7 @@
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1444,7 +1453,7 @@
         <v>8</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1464,10 +1473,10 @@
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
       <c r="J26" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1485,7 +1494,7 @@
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
       <c r="J27" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1536,10 +1545,10 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1557,7 +1566,7 @@
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
       <c r="J30" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1589,7 +1598,9 @@
         <f>C32 - E31</f>
         <v>0</v>
       </c>
-      <c r="J31" s="12"/>
+      <c r="J31" s="12" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
@@ -1608,10 +1619,10 @@
       <c r="H32" s="14"/>
       <c r="I32" s="14"/>
       <c r="J32" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -1629,7 +1640,7 @@
       <c r="H33" s="17"/>
       <c r="I33" s="17"/>
       <c r="J33" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -1680,10 +1691,10 @@
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1735,7 +1746,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" s="14" t="s">
         <v>2</v>
@@ -1750,7 +1761,7 @@
       <c r="H38" s="14"/>
       <c r="I38" s="14"/>
       <c r="J38" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2089,7 +2100,7 @@
         <v>726104</v>
       </c>
       <c r="J60" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -2194,7 +2205,7 @@
         <v>735452</v>
       </c>
       <c r="J66" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -2300,7 +2311,7 @@
         <v>735616</v>
       </c>
       <c r="J72" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
@@ -2355,7 +2366,7 @@
         <v>735688</v>
       </c>
       <c r="J75" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
@@ -2406,7 +2417,7 @@
         <v>735708</v>
       </c>
       <c r="J78" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -2457,7 +2468,7 @@
         <v>736020</v>
       </c>
       <c r="J81" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
@@ -2468,7 +2479,7 @@
         <v>200</v>
       </c>
       <c r="J82" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
@@ -2511,7 +2522,7 @@
         <v>833652</v>
       </c>
       <c r="J84" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
@@ -2562,7 +2573,7 @@
         <v>839460</v>
       </c>
       <c r="J87" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
@@ -2613,7 +2624,7 @@
         <v>839536</v>
       </c>
       <c r="J90" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
@@ -2712,7 +2723,7 @@
         <v>839752</v>
       </c>
       <c r="J96" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
@@ -2760,7 +2771,7 @@
         <v>975956</v>
       </c>
       <c r="J99" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
@@ -2771,7 +2782,7 @@
         <v>1</v>
       </c>
       <c r="J100" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
@@ -2814,7 +2825,7 @@
         <v>1049636</v>
       </c>
       <c r="J102" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
@@ -2865,7 +2876,7 @@
         <v>1049652</v>
       </c>
       <c r="J105" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
@@ -2997,7 +3008,7 @@
         <v>8</v>
       </c>
       <c r="I113" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Model compression and stuff
</commit_message>
<xml_diff>
--- a/Research/BSP Layout.xlsx
+++ b/Research/BSP Layout.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ron\Desktop\openh2\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2926F6-1BCD-4C34-8C5E-9B4A86B764EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7D2066-5284-465D-9A27-ADEC6FDA231D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34035" yWindow="2310" windowWidth="21600" windowHeight="11505" xr2:uid="{7C22A468-B651-4234-BD2F-70F5ECA787F1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{7C22A468-B651-4234-BD2F-70F5ECA787F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="86">
   <si>
     <t>File size</t>
   </si>
@@ -244,13 +245,58 @@
   </si>
   <si>
     <t>Clusters/render chunks</t>
+  </si>
+  <si>
+    <t>Cao Location</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Description/notes</t>
+  </si>
+  <si>
+    <t>shader tags</t>
+  </si>
+  <si>
+    <t>RealOffset</t>
+  </si>
+  <si>
+    <t>mostly a lot of floats</t>
+  </si>
+  <si>
+    <t>decals</t>
+  </si>
+  <si>
+    <t>garbage</t>
+  </si>
+  <si>
+    <t>Collision geometry</t>
+  </si>
+  <si>
+    <t>Render chunks</t>
+  </si>
+  <si>
+    <t>Shaders</t>
+  </si>
+  <si>
+    <t>sound string/tag refs</t>
+  </si>
+  <si>
+    <t>sound effect string/tag refs</t>
+  </si>
+  <si>
+    <t>portals?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,8 +319,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,6 +361,16 @@
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -553,12 +623,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -585,9 +657,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1000,7 +1076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5402844C-0554-4902-B07C-5C11243F8396}">
   <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
@@ -3024,4 +3100,738 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63038823-1BD4-4E0D-A55E-E822A9D37B5E}">
+  <dimension ref="B1:M30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="88.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>36</v>
+      </c>
+      <c r="D2">
+        <v>572</v>
+      </c>
+      <c r="E2">
+        <f>D2 +42332576</f>
+        <v>42333148</v>
+      </c>
+      <c r="F2">
+        <f>(D3-D2)/C2</f>
+        <v>20</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" ref="I2:I14" si="0">"[FixedLength(" &amp; F2 &amp; ")]public class Obj" &amp; B2 &amp; " {}"</f>
+        <v>[FixedLength(20)]public class Obj12 {}</v>
+      </c>
+      <c r="M2" t="str">
+        <f t="shared" ref="M2:M14" si="1">"[InternalReferenceValue(" &amp; B2 &amp; ")] public Obj" &amp; B2 &amp; "[] Obj" &amp; B2 &amp; "s { get; set; }"</f>
+        <v>[InternalReferenceValue(12)] public Obj12[] Obj12s { get; set; }</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1292</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E30" si="2">D3 +42332576</f>
+        <v>42333868</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F30" si="3">(D4-D3)/C3</f>
+        <v>610532</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" si="0"/>
+        <v>[FixedLength(610532)]public class Obj20 {}</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" si="1"/>
+        <v>[InternalReferenceValue(20)] public Obj20[] Obj20s { get; set; }</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>44</v>
+      </c>
+      <c r="C4">
+        <v>5427</v>
+      </c>
+      <c r="D4">
+        <v>611824</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>42944400</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>[FixedLength(8)]public class Obj44 {}</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="1"/>
+        <v>[InternalReferenceValue(44)] public Obj44[] Obj44s { get; set; }</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>76</v>
+      </c>
+      <c r="C5">
+        <v>23580</v>
+      </c>
+      <c r="D5">
+        <v>655240</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>42987816</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>[FixedLength(8)]public class Obj76 {}</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="1"/>
+        <v>[InternalReferenceValue(76)] public Obj76[] Obj76s { get; set; }</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>84</v>
+      </c>
+      <c r="C6">
+        <v>880</v>
+      </c>
+      <c r="D6">
+        <v>843880</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>43176456</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>[FixedLength(1)]public class Obj84 {}</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="1"/>
+        <v>[InternalReferenceValue(84)] public Obj84[] Obj84s { get; set; }</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>92</v>
+      </c>
+      <c r="C7">
+        <v>125</v>
+      </c>
+      <c r="D7">
+        <v>844760</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>43177336</v>
+      </c>
+      <c r="F7">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>[FixedLength(36)]public class Obj92 {}</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="1"/>
+        <v>[InternalReferenceValue(92)] public Obj92[] Obj92s { get; set; }</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>857696</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>43190272</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>[FixedLength(24)]public class Obj100 {}</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="1"/>
+        <v>[InternalReferenceValue(100)] public Obj100[] Obj100s { get; set; }</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>148</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>857720</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>43190296</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>[FixedLength(36)]public class Obj148 {}</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="1"/>
+        <v>[InternalReferenceValue(148)] public Obj148[] Obj148s { get; set; }</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>156</v>
+      </c>
+      <c r="C10">
+        <v>55</v>
+      </c>
+      <c r="D10">
+        <v>857756</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>43190332</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="3"/>
+        <v>612.29090909090905</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>[FixedLength(612.290909090909)]public class Obj156 {}</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="1"/>
+        <v>[InternalReferenceValue(156)] public Obj156[] Obj156s { get; set; }</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>164</v>
+      </c>
+      <c r="C11">
+        <v>93</v>
+      </c>
+      <c r="D11">
+        <v>891432</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>43224008</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="3"/>
+        <v>34.322580645161288</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>[FixedLength(34.3225806451613)]public class Obj164 {}</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="1"/>
+        <v>[InternalReferenceValue(164)] public Obj164[] Obj164s { get; set; }</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>172</v>
+      </c>
+      <c r="C12">
+        <v>32</v>
+      </c>
+      <c r="D12">
+        <v>894624</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>43227200</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>[FixedLength(2)]public class Obj172 {}</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="1"/>
+        <v>[InternalReferenceValue(172)] public Obj172[] Obj172s { get; set; }</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>212</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>894688</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>43227264</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="G13" t="s">
+        <v>83</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>[FixedLength(100)]public class Obj212 {}</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="1"/>
+        <v>[InternalReferenceValue(212)] public Obj212[] Obj212s { get; set; }</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>220</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>895088</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>43227664</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+      <c r="G14" t="s">
+        <v>84</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>[FixedLength(72)]public class Obj220 {}</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="1"/>
+        <v>[InternalReferenceValue(220)] public Obj220[] Obj220s { get; set; }</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>244</v>
+      </c>
+      <c r="C15">
+        <v>40</v>
+      </c>
+      <c r="D15">
+        <v>895232</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>43227808</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="I15" t="str">
+        <f>"[FixedLength(" &amp; F15 &amp; ")]public class Obj" &amp; B15 &amp; " {}"</f>
+        <v>[FixedLength(16)]public class Obj244 {}</v>
+      </c>
+      <c r="M15" t="str">
+        <f>"[InternalReferenceValue(" &amp; B15 &amp; ")] public Obj" &amp; B15 &amp; "[] Obj" &amp; B15 &amp; "s { get; set; }"</f>
+        <v>[InternalReferenceValue(244)] public Obj244[] Obj244s { get; set; }</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>252</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>895872</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>43228448</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>260</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>895892</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>43228468</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="3"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>312</v>
+      </c>
+      <c r="C18">
+        <v>19</v>
+      </c>
+      <c r="D18">
+        <v>896204</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>43228780</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="3"/>
+        <v>11916.421052631578</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>320</v>
+      </c>
+      <c r="C19">
+        <v>62</v>
+      </c>
+      <c r="D19">
+        <v>1122616</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>43455192</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="3"/>
+        <v>88</v>
+      </c>
+      <c r="G19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>328</v>
+      </c>
+      <c r="C20">
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>1128072</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>43460648</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="3"/>
+        <v>69.777777777777771</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>336</v>
+      </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <v>1128700</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>43461276</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="3"/>
+        <v>68.888888888888886</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>344</v>
+      </c>
+      <c r="C22">
+        <v>34</v>
+      </c>
+      <c r="D22">
+        <v>1129320</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>43461896</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>464</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1130000</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>43462576</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="3"/>
+        <v>58048</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>480</v>
+      </c>
+      <c r="C24">
+        <v>85696</v>
+      </c>
+      <c r="D24">
+        <v>1188048</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>43520624</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>516</v>
+      </c>
+      <c r="C25">
+        <v>288</v>
+      </c>
+      <c r="D25">
+        <v>1273744</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>43606320</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>524</v>
+      </c>
+      <c r="C26">
+        <v>27</v>
+      </c>
+      <c r="D26">
+        <v>1274032</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>43606608</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>532</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1274896</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>43607472</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="3"/>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>540</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1275116</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>43607692</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>548</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1275132</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>43607708</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="3"/>
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>564</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1276860</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>43609436</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="3"/>
+        <v>-1276860</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adds alpha texture usage
</commit_message>
<xml_diff>
--- a/Research/BSP Layout.xlsx
+++ b/Research/BSP Layout.xlsx
@@ -1,21 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ron\Desktop\openh2\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7D2066-5284-465D-9A27-ADEC6FDA231D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5209C5A8-76DA-478E-A77C-2F6FFC69BBE6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{7C22A468-B651-4234-BD2F-70F5ECA787F1}"/>
+    <workbookView xWindow="30375" yWindow="345" windowWidth="26160" windowHeight="13995" firstSheet="2" activeTab="2" xr2:uid="{7C22A468-B651-4234-BD2F-70F5ECA787F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="ascension" sheetId="2" r:id="rId2"/>
+    <sheet name="zanzibar" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="MixedRefs">[1]Sheet1!$B$2:$F$61</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="115">
   <si>
     <t>File size</t>
   </si>
@@ -290,6 +298,93 @@
   </si>
   <si>
     <t>portals?</t>
+  </si>
+  <si>
+    <t>shaders</t>
+  </si>
+  <si>
+    <t>collision</t>
+  </si>
+  <si>
+    <t>renderchunks</t>
+  </si>
+  <si>
+    <t>{short, short, uint}</t>
+  </si>
+  <si>
+    <t>{int, short, short}?</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>{short, short float[4]}</t>
+  </si>
+  <si>
+    <t>zero</t>
+  </si>
+  <si>
+    <t>more shader references</t>
+  </si>
+  <si>
+    <t>FFx64</t>
+  </si>
+  <si>
+    <t>Name and lsnd references</t>
+  </si>
+  <si>
+    <t>Name and snde references</t>
+  </si>
+  <si>
+    <t>null scen and mode reference</t>
+  </si>
+  <si>
+    <t>Name, floats, referencing machines flywheel instances</t>
+  </si>
+  <si>
+    <t>not sure</t>
+  </si>
+  <si>
+    <t>Index, then 2? Internal references</t>
+  </si>
+  <si>
+    <t>Sparse section of internal references, then data</t>
+  </si>
+  <si>
+    <t>Decal</t>
+  </si>
+  <si>
+    <t>{short, short, float[4]} - not positional info</t>
+  </si>
+  <si>
+    <t>4 shorts, 6 floats - floats do not appear positional</t>
+  </si>
+  <si>
+    <t>CaoOffset</t>
+  </si>
+  <si>
+    <t>Absolute</t>
+  </si>
+  <si>
+    <t>Internal magic:</t>
+  </si>
+  <si>
+    <t>portals? - probably…?, I'm thinking the last reference points to verticies in polygon defining</t>
+  </si>
+  <si>
+    <t>Instanced Geometry instances</t>
+  </si>
+  <si>
+    <t>instanced geom defs…? Yes...?</t>
+  </si>
+  <si>
+    <t>Geom def magic:</t>
+  </si>
+  <si>
+    <t>val:</t>
+  </si>
+  <si>
+    <t>Sec magic</t>
   </si>
 </sst>
 </file>
@@ -758,6 +853,870 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Sheet2 (2)"/>
+      <sheetName val="Sheet4"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="B2">
+            <v>8</v>
+          </cell>
+          <cell r="C2">
+            <v>1</v>
+          </cell>
+          <cell r="D2">
+            <v>992</v>
+          </cell>
+          <cell r="E2">
+            <v>8</v>
+          </cell>
+          <cell r="F2" t="str">
+            <v>Skybox refs</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3">
+            <v>72</v>
+          </cell>
+          <cell r="C3">
+            <v>1</v>
+          </cell>
+          <cell r="D3">
+            <v>1000</v>
+          </cell>
+          <cell r="E3">
+            <v>36</v>
+          </cell>
+          <cell r="F3" t="str">
+            <v>mostly empty, last 4 bytes is two shorts, [6,2]</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4">
+            <v>80</v>
+          </cell>
+          <cell r="C4">
+            <v>7</v>
+          </cell>
+          <cell r="D4">
+            <v>1036</v>
+          </cell>
+          <cell r="E4">
+            <v>92</v>
+          </cell>
+          <cell r="F4" t="str">
+            <v>scenery</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5">
+            <v>88</v>
+          </cell>
+          <cell r="C5">
+            <v>10</v>
+          </cell>
+          <cell r="D5">
+            <v>1680</v>
+          </cell>
+          <cell r="E5">
+            <v>40</v>
+          </cell>
+          <cell r="F5" t="str">
+            <v>Scen tag references, padded with zeroes</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>152</v>
+          </cell>
+          <cell r="C6">
+            <v>5</v>
+          </cell>
+          <cell r="D6">
+            <v>2080</v>
+          </cell>
+          <cell r="E6">
+            <v>40</v>
+          </cell>
+          <cell r="F6" t="str">
+            <v>Weap tag references, padded with zeroes</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>168</v>
+          </cell>
+          <cell r="C7">
+            <v>4</v>
+          </cell>
+          <cell r="D7">
+            <v>2280</v>
+          </cell>
+          <cell r="E7">
+            <v>72</v>
+          </cell>
+          <cell r="F7" t="str">
+            <v>definitely sword placement on zanzibar - but not on lockout, no shotgun on lockout either</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>176</v>
+          </cell>
+          <cell r="C8">
+            <v>3</v>
+          </cell>
+          <cell r="D8">
+            <v>2568</v>
+          </cell>
+          <cell r="E8">
+            <v>40</v>
+          </cell>
+          <cell r="F8" t="str">
+            <v>Mach tag references, padded with zeroes</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9">
+            <v>216</v>
+          </cell>
+          <cell r="C9">
+            <v>1</v>
+          </cell>
+          <cell r="D9">
+            <v>2688</v>
+          </cell>
+          <cell r="E9">
+            <v>80</v>
+          </cell>
+          <cell r="F9" t="str">
+            <v>Ssce placement?</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10">
+            <v>224</v>
+          </cell>
+          <cell r="C10">
+            <v>2</v>
+          </cell>
+          <cell r="D10">
+            <v>2768</v>
+          </cell>
+          <cell r="E10">
+            <v>40</v>
+          </cell>
+          <cell r="F10" t="str">
+            <v>Ssce tag references, padded with zeroes</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11">
+            <v>232</v>
+          </cell>
+          <cell r="C11">
+            <v>2</v>
+          </cell>
+          <cell r="D11">
+            <v>2848</v>
+          </cell>
+          <cell r="E11">
+            <v>108</v>
+          </cell>
+          <cell r="F11" t="str">
+            <v>Light placement?</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12">
+            <v>240</v>
+          </cell>
+          <cell r="C12">
+            <v>1</v>
+          </cell>
+          <cell r="D12">
+            <v>3064</v>
+          </cell>
+          <cell r="E12">
+            <v>40</v>
+          </cell>
+          <cell r="F12" t="str">
+            <v>Ligh tag reference, padded with zeroes</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13">
+            <v>256</v>
+          </cell>
+          <cell r="C13">
+            <v>68</v>
+          </cell>
+          <cell r="D13">
+            <v>3104</v>
+          </cell>
+          <cell r="E13">
+            <v>52</v>
+          </cell>
+          <cell r="F13" t="str">
+            <v>player spawn, xyz with rotation - almost certainly</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14">
+            <v>264</v>
+          </cell>
+          <cell r="C14">
+            <v>4</v>
+          </cell>
+          <cell r="D14">
+            <v>6640</v>
+          </cell>
+          <cell r="E14">
+            <v>68</v>
+          </cell>
+          <cell r="F14" t="str">
+            <v>byte sized enums/indicies, zeroes, and six floats</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15">
+            <v>280</v>
+          </cell>
+          <cell r="C15">
+            <v>84</v>
+          </cell>
+          <cell r="D15">
+            <v>6912</v>
+          </cell>
+          <cell r="E15">
+            <v>32</v>
+          </cell>
+          <cell r="F15" t="str">
+            <v>game mode markers? KotH, Flag spawns, etc</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="B16">
+            <v>288</v>
+          </cell>
+          <cell r="C16">
+            <v>33</v>
+          </cell>
+          <cell r="D16">
+            <v>9600</v>
+          </cell>
+          <cell r="E16">
+            <v>144</v>
+          </cell>
+          <cell r="F16" t="str">
+            <v>Itmc references, flags, zeroes, xyz, orientation, and tag id</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17">
+            <v>296</v>
+          </cell>
+          <cell r="C17">
+            <v>1</v>
+          </cell>
+          <cell r="D17">
+            <v>14352</v>
+          </cell>
+          <cell r="E17">
+            <v>156</v>
+          </cell>
+          <cell r="F17" t="str">
+            <v>Itmc refs, all null tag except first - default equip?</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="B18">
+            <v>320</v>
+          </cell>
+          <cell r="C18">
+            <v>6</v>
+          </cell>
+          <cell r="D18">
+            <v>14508</v>
+          </cell>
+          <cell r="E18">
+            <v>8</v>
+          </cell>
+          <cell r="F18" t="str">
+            <v>Deca references, tight</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="B19">
+            <v>432</v>
+          </cell>
+          <cell r="C19">
+            <v>1024</v>
+          </cell>
+          <cell r="D19">
+            <v>14556</v>
+          </cell>
+          <cell r="E19">
+            <v>1</v>
+          </cell>
+          <cell r="F19" t="str">
+            <v>Text</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="B20">
+            <v>472</v>
+          </cell>
+          <cell r="C20">
+            <v>1</v>
+          </cell>
+          <cell r="D20">
+            <v>15580</v>
+          </cell>
+          <cell r="E20">
+            <v>128</v>
+          </cell>
+          <cell r="F20" t="str">
+            <v>All zeroes</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="B21">
+            <v>528</v>
+          </cell>
+          <cell r="C21">
+            <v>1</v>
+          </cell>
+          <cell r="D21">
+            <v>15708</v>
+          </cell>
+          <cell r="E21">
+            <v>68</v>
+          </cell>
+          <cell r="F21" t="str">
+            <v>Sbsp and lightmap tag references, maybe some flags</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="B22">
+            <v>536</v>
+          </cell>
+          <cell r="C22">
+            <v>1</v>
+          </cell>
+          <cell r="D22">
+            <v>15776</v>
+          </cell>
+          <cell r="E22">
+            <v>152</v>
+          </cell>
+          <cell r="F22" t="str">
+            <v>Internal ref to a series of tag refs -&gt; *cen, *piq, refs, etc</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="B23">
+            <v>560</v>
+          </cell>
+          <cell r="C23">
+            <v>4</v>
+          </cell>
+          <cell r="D23">
+            <v>15928</v>
+          </cell>
+          <cell r="E23">
+            <v>2</v>
+          </cell>
+          <cell r="F23" t="str">
+            <v>Ids as shorts?</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="B24">
+            <v>568</v>
+          </cell>
+          <cell r="C24">
+            <v>515</v>
+          </cell>
+          <cell r="D24">
+            <v>15936</v>
+          </cell>
+          <cell r="E24">
+            <v>20</v>
+          </cell>
+          <cell r="F24" t="str">
+            <v>Just 00, then 16 bytes of BA</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25">
+            <v>592</v>
+          </cell>
+          <cell r="C25">
+            <v>1</v>
+          </cell>
+          <cell r="D25">
+            <v>26236</v>
+          </cell>
+          <cell r="E25">
+            <v>100</v>
+          </cell>
+          <cell r="F25" t="str">
+            <v>ascension string, then zeroes, then lsnd ref</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26">
+            <v>600</v>
+          </cell>
+          <cell r="C26">
+            <v>1</v>
+          </cell>
+          <cell r="D26">
+            <v>26336</v>
+          </cell>
+          <cell r="E26">
+            <v>72</v>
+          </cell>
+          <cell r="F26" t="str">
+            <v>cliffs string, snde reference</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27">
+            <v>656</v>
+          </cell>
+          <cell r="C27">
+            <v>1</v>
+          </cell>
+          <cell r="D27">
+            <v>26408</v>
+          </cell>
+          <cell r="E27">
+            <v>192</v>
+          </cell>
+          <cell r="F27" t="str">
+            <v>Null sbsp tagref, internal refs to subsequent values (floats)</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28">
+            <v>792</v>
+          </cell>
+          <cell r="C28">
+            <v>1</v>
+          </cell>
+          <cell r="D28">
+            <v>26600</v>
+          </cell>
+          <cell r="E28">
+            <v>816</v>
+          </cell>
+          <cell r="F28" t="str">
+            <v>Internal refs, 48 size blocks, then more 48 size blocks. Lots of floats</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="B29">
+            <v>808</v>
+          </cell>
+          <cell r="C29">
+            <v>1</v>
+          </cell>
+          <cell r="D29">
+            <v>27416</v>
+          </cell>
+          <cell r="E29">
+            <v>76</v>
+          </cell>
+          <cell r="F29" t="str">
+            <v>Crates and stuff</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="B30">
+            <v>816</v>
+          </cell>
+          <cell r="C30">
+            <v>1</v>
+          </cell>
+          <cell r="D30">
+            <v>27492</v>
+          </cell>
+          <cell r="E30">
+            <v>40</v>
+          </cell>
+          <cell r="F30" t="str">
+            <v>bloc ref, padded with zeroes</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="B31">
+            <v>840</v>
+          </cell>
+          <cell r="C31">
+            <v>1</v>
+          </cell>
+          <cell r="D31">
+            <v>27532</v>
+          </cell>
+          <cell r="E31">
+            <v>16</v>
+          </cell>
+          <cell r="F31" t="str">
+            <v>Fog tag - ref?</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="B32">
+            <v>904</v>
+          </cell>
+          <cell r="C32">
+            <v>1</v>
+          </cell>
+          <cell r="D32">
+            <v>27548</v>
+          </cell>
+          <cell r="E32">
+            <v>16</v>
+          </cell>
+          <cell r="F32" t="str">
+            <v>Empty sbsp ref</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="B33">
+            <v>920</v>
+          </cell>
+          <cell r="C33">
+            <v>1</v>
+          </cell>
+          <cell r="D33">
+            <v>27564</v>
+          </cell>
+          <cell r="E33">
+            <v>3196</v>
+          </cell>
+          <cell r="F33" t="str">
+            <v>Bitm, then utf-16 strings of the name and description of the map</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="B34">
+            <v>984</v>
+          </cell>
+          <cell r="C34">
+            <v>344</v>
+          </cell>
+          <cell r="D34">
+            <v>30760</v>
+          </cell>
+          <cell r="E34">
+            <v>4</v>
+          </cell>
+          <cell r="F34" t="str">
+            <v>Shorts referencing the current raw offset. Padding for future changes to prevent recalculating magics?</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="D35">
+            <v>32136</v>
+          </cell>
+          <cell r="F35" t="str">
+            <v>EOF</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="B39">
+            <v>96</v>
+          </cell>
+          <cell r="C39">
+            <v>2</v>
+          </cell>
+          <cell r="D39">
+            <v>5772</v>
+          </cell>
+          <cell r="E39">
+            <v>84</v>
+          </cell>
+          <cell r="F39" t="str">
+            <v>[1,9]/[0,10] then four floats, plus some other data</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="B40">
+            <v>104</v>
+          </cell>
+          <cell r="C40">
+            <v>2</v>
+          </cell>
+          <cell r="D40">
+            <v>5940</v>
+          </cell>
+          <cell r="E40">
+            <v>40</v>
+          </cell>
+          <cell r="F40" t="str">
+            <v>Bipd references</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="B41">
+            <v>144</v>
+          </cell>
+          <cell r="C41">
+            <v>1</v>
+          </cell>
+          <cell r="D41">
+            <v>6020</v>
+          </cell>
+          <cell r="E41">
+            <v>84</v>
+          </cell>
+          <cell r="F41" t="str">
+            <v>floats</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="B42">
+            <v>152</v>
+          </cell>
+          <cell r="C42">
+            <v>1</v>
+          </cell>
+          <cell r="D42">
+            <v>6104</v>
+          </cell>
+          <cell r="E42">
+            <v>40</v>
+          </cell>
+          <cell r="F42" t="str">
+            <v>weap ref</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="B43">
+            <v>160</v>
+          </cell>
+          <cell r="C43">
+            <v>1</v>
+          </cell>
+          <cell r="D43">
+            <v>6144</v>
+          </cell>
+          <cell r="E43">
+            <v>40</v>
+          </cell>
+          <cell r="F43" t="str">
+            <v>gate string</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="B44">
+            <v>168</v>
+          </cell>
+          <cell r="C44">
+            <v>6</v>
+          </cell>
+          <cell r="D44">
+            <v>6184</v>
+          </cell>
+          <cell r="E44">
+            <v>72</v>
+          </cell>
+          <cell r="F44" t="str">
+            <v>floats</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="B45">
+            <v>176</v>
+          </cell>
+          <cell r="C45">
+            <v>4</v>
+          </cell>
+          <cell r="D45">
+            <v>6616</v>
+          </cell>
+          <cell r="E45">
+            <v>40</v>
+          </cell>
+          <cell r="F45" t="str">
+            <v>machine references</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="B46">
+            <v>184</v>
+          </cell>
+          <cell r="C46">
+            <v>1</v>
+          </cell>
+          <cell r="D46">
+            <v>6776</v>
+          </cell>
+          <cell r="E46">
+            <v>68</v>
+          </cell>
+          <cell r="F46" t="str">
+            <v>floats - ctrl placement</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="B47">
+            <v>192</v>
+          </cell>
+          <cell r="C47">
+            <v>1</v>
+          </cell>
+          <cell r="D47">
+            <v>6844</v>
+          </cell>
+          <cell r="E47">
+            <v>40</v>
+          </cell>
+          <cell r="F47" t="str">
+            <v>ctrl ref</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="D48">
+            <v>6884</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="B50">
+            <v>312</v>
+          </cell>
+          <cell r="C50">
+            <v>40</v>
+          </cell>
+          <cell r="D50">
+            <v>26256</v>
+          </cell>
+          <cell r="E50">
+            <v>16</v>
+          </cell>
+          <cell r="F50" t="str">
+            <v>decal placements</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="D51">
+            <v>26896</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="B53">
+            <v>440</v>
+          </cell>
+          <cell r="C53">
+            <v>24</v>
+          </cell>
+          <cell r="D53">
+            <v>29172</v>
+          </cell>
+          <cell r="E53">
+            <v>40</v>
+          </cell>
+          <cell r="F53" t="str">
+            <v>text with refs</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="B54">
+            <v>448</v>
+          </cell>
+          <cell r="C54">
+            <v>1</v>
+          </cell>
+          <cell r="D54">
+            <v>30132</v>
+          </cell>
+          <cell r="E54">
+            <v>40</v>
+          </cell>
+          <cell r="F54" t="str">
+            <v>same as above</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="D55">
+            <v>30172</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="B57">
+            <v>480</v>
+          </cell>
+          <cell r="C57">
+            <v>6</v>
+          </cell>
+          <cell r="D57">
+            <v>30300</v>
+          </cell>
+          <cell r="E57">
+            <v>56</v>
+          </cell>
+          <cell r="F57" t="str">
+            <v>strings with floats</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="B58">
+            <v>488</v>
+          </cell>
+          <cell r="C58">
+            <v>49</v>
+          </cell>
+          <cell r="D58">
+            <v>30636</v>
+          </cell>
+          <cell r="E58">
+            <v>64</v>
+          </cell>
+          <cell r="F58" t="str">
+            <v>strings, floats</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="D59">
+            <v>33772</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="B61">
+            <v>888</v>
+          </cell>
+          <cell r="C61">
+            <v>2</v>
+          </cell>
+          <cell r="D61">
+            <v>66896</v>
+          </cell>
+          <cell r="E61">
+            <v>8</v>
+          </cell>
+          <cell r="F61" t="str">
+            <v>DECR refs</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4A306544-E06B-4C2F-8FD8-9914D7356CDF}" name="Table2" displayName="Table2" ref="A44:J113" totalsRowShown="0">
   <autoFilter ref="A44:J113" xr:uid="{EF8F3AD4-1BC3-4A9C-9CBD-813263F6B0E9}"/>
@@ -1076,8 +2035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5402844C-0554-4902-B07C-5C11243F8396}">
   <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J60" sqref="J60"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3106,8 +4065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63038823-1BD4-4E0D-A55E-E822A9D37B5E}">
   <dimension ref="B1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3143,7 +4102,7 @@
         <v>12</v>
       </c>
       <c r="C2">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>572</v>
@@ -3176,22 +4135,22 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1292</v>
+        <v>912</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E30" si="2">D3 +42332576</f>
-        <v>42333868</v>
+        <v>42333488</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F30" si="3">(D4-D3)/C3</f>
-        <v>610532</v>
+        <v>515540</v>
       </c>
       <c r="G3" s="25" t="s">
         <v>80</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" si="0"/>
-        <v>[FixedLength(610532)]public class Obj20 {}</v>
+        <v>[FixedLength(515540)]public class Obj20 {}</v>
       </c>
       <c r="M3" t="str">
         <f t="shared" si="1"/>
@@ -3203,14 +4162,14 @@
         <v>44</v>
       </c>
       <c r="C4">
-        <v>5427</v>
+        <v>6596</v>
       </c>
       <c r="D4">
-        <v>611824</v>
+        <v>516452</v>
       </c>
       <c r="E4">
         <f t="shared" si="2"/>
-        <v>42944400</v>
+        <v>42849028</v>
       </c>
       <c r="F4">
         <f t="shared" si="3"/>
@@ -3230,14 +4189,14 @@
         <v>76</v>
       </c>
       <c r="C5">
-        <v>23580</v>
+        <v>19365</v>
       </c>
       <c r="D5">
-        <v>655240</v>
+        <v>569220</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
-        <v>42987816</v>
+        <v>42901796</v>
       </c>
       <c r="F5">
         <f t="shared" si="3"/>
@@ -3257,14 +4216,14 @@
         <v>84</v>
       </c>
       <c r="C6">
-        <v>880</v>
+        <v>56</v>
       </c>
       <c r="D6">
-        <v>843880</v>
+        <v>724140</v>
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
-        <v>43176456</v>
+        <v>43056716</v>
       </c>
       <c r="F6">
         <f t="shared" si="3"/>
@@ -3284,14 +4243,14 @@
         <v>92</v>
       </c>
       <c r="C7">
-        <v>125</v>
+        <v>19</v>
       </c>
       <c r="D7">
-        <v>844760</v>
+        <v>724196</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
-        <v>43177336</v>
+        <v>43056772</v>
       </c>
       <c r="F7">
         <v>36</v>
@@ -3316,11 +4275,11 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>857696</v>
+        <v>726044</v>
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
-        <v>43190272</v>
+        <v>43058620</v>
       </c>
       <c r="F8">
         <f t="shared" si="3"/>
@@ -3343,11 +4302,11 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>857720</v>
+        <v>726068</v>
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
-        <v>43190296</v>
+        <v>43058644</v>
       </c>
       <c r="F9">
         <f t="shared" si="3"/>
@@ -3367,25 +4326,25 @@
         <v>156</v>
       </c>
       <c r="C10">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="D10">
-        <v>857756</v>
+        <v>726104</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>43190332</v>
+        <v>43058680</v>
       </c>
       <c r="F10">
         <f t="shared" si="3"/>
-        <v>612.29090909090905</v>
+        <v>1065.7142857142858</v>
       </c>
       <c r="G10" s="25" t="s">
         <v>81</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
-        <v>[FixedLength(612.290909090909)]public class Obj156 {}</v>
+        <v>[FixedLength(1065.71428571429)]public class Obj156 {}</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="1"/>
@@ -3397,25 +4356,25 @@
         <v>164</v>
       </c>
       <c r="C11">
-        <v>93</v>
+        <v>53</v>
       </c>
       <c r="D11">
-        <v>891432</v>
+        <v>733564</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>43224008</v>
+        <v>43066140</v>
       </c>
       <c r="F11">
         <f t="shared" si="3"/>
-        <v>34.322580645161288</v>
+        <v>35.622641509433961</v>
       </c>
       <c r="G11" s="25" t="s">
         <v>82</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
-        <v>[FixedLength(34.3225806451613)]public class Obj164 {}</v>
+        <v>[FixedLength(35.622641509434)]public class Obj164 {}</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="1"/>
@@ -3430,11 +4389,11 @@
         <v>32</v>
       </c>
       <c r="D12">
-        <v>894624</v>
+        <v>735452</v>
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>43227200</v>
+        <v>43068028</v>
       </c>
       <c r="F12">
         <f t="shared" si="3"/>
@@ -3457,14 +4416,14 @@
         <v>212</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>894688</v>
+        <v>735516</v>
       </c>
       <c r="E13">
         <f t="shared" si="2"/>
-        <v>43227264</v>
+        <v>43068092</v>
       </c>
       <c r="F13">
         <f t="shared" si="3"/>
@@ -3487,14 +4446,14 @@
         <v>220</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>895088</v>
+        <v>735616</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>43227664</v>
+        <v>43068192</v>
       </c>
       <c r="F14">
         <f t="shared" si="3"/>
@@ -3514,324 +4473,1294 @@
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="C15">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>895232</v>
+        <v>735688</v>
       </c>
       <c r="E15">
         <f t="shared" si="2"/>
-        <v>43227808</v>
+        <v>43068264</v>
       </c>
       <c r="F15">
         <f t="shared" si="3"/>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G15" s="25" t="s">
         <v>78</v>
       </c>
       <c r="I15" t="str">
         <f>"[FixedLength(" &amp; F15 &amp; ")]public class Obj" &amp; B15 &amp; " {}"</f>
-        <v>[FixedLength(16)]public class Obj244 {}</v>
+        <v>[FixedLength(20)]public class Obj252 {}</v>
       </c>
       <c r="M15" t="str">
         <f>"[InternalReferenceValue(" &amp; B15 &amp; ")] public Obj" &amp; B15 &amp; "[] Obj" &amp; B15 &amp; "s { get; set; }"</f>
-        <v>[InternalReferenceValue(244)] public Obj244[] Obj244s { get; set; }</v>
+        <v>[InternalReferenceValue(252)] public Obj252[] Obj252s { get; set; }</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>895872</v>
+        <v>735708</v>
       </c>
       <c r="E16">
         <f t="shared" si="2"/>
-        <v>43228448</v>
+        <v>43068284</v>
       </c>
       <c r="F16">
         <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" ref="I16:I30" si="4">"[FixedLength(" &amp; F16 &amp; ")]public class Obj" &amp; B16 &amp; " {}"</f>
+        <v>[FixedLength(104)]public class Obj260 {}</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" ref="M16:M30" si="5">"[InternalReferenceValue(" &amp; B16 &amp; ")] public Obj" &amp; B16 &amp; "[] Obj" &amp; B16 &amp; "s { get; set; }"</f>
+        <v>[InternalReferenceValue(260)] public Obj260[] Obj260s { get; set; }</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>260</v>
+        <v>312</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D17">
-        <v>895892</v>
+        <v>736020</v>
       </c>
       <c r="E17">
         <f t="shared" si="2"/>
-        <v>43228468</v>
+        <v>43068596</v>
       </c>
       <c r="F17">
         <f t="shared" si="3"/>
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+        <v>5138.5263157894733</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="4"/>
+        <v>[FixedLength(5138.52631578947)]public class Obj312 {}</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="5"/>
+        <v>[InternalReferenceValue(312)] public Obj312[] Obj312s { get; set; }</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="C18">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="D18">
-        <v>896204</v>
+        <v>833652</v>
       </c>
       <c r="E18">
         <f t="shared" si="2"/>
-        <v>43228780</v>
+        <v>43166228</v>
       </c>
       <c r="F18">
         <f t="shared" si="3"/>
-        <v>11916.421052631578</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="4"/>
+        <v>[FixedLength(88)]public class Obj320 {}</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="5"/>
+        <v>[InternalReferenceValue(320)] public Obj320[] Obj320s { get; set; }</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="C19">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>1122616</v>
+        <v>839460</v>
       </c>
       <c r="E19">
         <f t="shared" si="2"/>
-        <v>43455192</v>
+        <v>43172036</v>
       </c>
       <c r="F19">
         <f t="shared" si="3"/>
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="G19" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I19" t="str">
+        <f t="shared" si="4"/>
+        <v>[FixedLength(76)]public class Obj328 {}</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="5"/>
+        <v>[InternalReferenceValue(328)] public Obj328[] Obj328s { get; set; }</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>328</v>
+        <v>336</v>
       </c>
       <c r="C20">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>1128072</v>
+        <v>839536</v>
       </c>
       <c r="E20">
         <f t="shared" si="2"/>
-        <v>43460648</v>
+        <v>43172112</v>
       </c>
       <c r="F20">
         <f t="shared" si="3"/>
-        <v>69.777777777777771</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="4"/>
+        <v>[FixedLength(76)]public class Obj336 {}</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="5"/>
+        <v>[InternalReferenceValue(336)] public Obj336[] Obj336s { get; set; }</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="C21">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D21">
-        <v>1128700</v>
+        <v>839612</v>
       </c>
       <c r="E21">
         <f t="shared" si="2"/>
-        <v>43461276</v>
+        <v>43172188</v>
       </c>
       <c r="F21">
         <f t="shared" si="3"/>
-        <v>68.888888888888886</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="4"/>
+        <v>[FixedLength(20)]public class Obj344 {}</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="5"/>
+        <v>[InternalReferenceValue(344)] public Obj344[] Obj344s { get; set; }</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>344</v>
+        <v>464</v>
       </c>
       <c r="C22">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>1129320</v>
+        <v>839752</v>
       </c>
       <c r="E22">
         <f t="shared" si="2"/>
-        <v>43461896</v>
+        <v>43172328</v>
       </c>
       <c r="F22">
         <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+        <v>136204</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="4"/>
+        <v>[FixedLength(136204)]public class Obj464 {}</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="5"/>
+        <v>[InternalReferenceValue(464)] public Obj464[] Obj464s { get; set; }</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>464</v>
+        <v>480</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>73680</v>
       </c>
       <c r="D23">
-        <v>1130000</v>
+        <v>975956</v>
       </c>
       <c r="E23">
         <f t="shared" si="2"/>
-        <v>43462576</v>
+        <v>43308532</v>
       </c>
       <c r="F23">
         <f t="shared" si="3"/>
-        <v>58048</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="4"/>
+        <v>[FixedLength(1)]public class Obj480 {}</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="5"/>
+        <v>[InternalReferenceValue(480)] public Obj480[] Obj480s { get; set; }</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>480</v>
+        <v>540</v>
       </c>
       <c r="C24">
-        <v>85696</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>1188048</v>
+        <v>1049636</v>
       </c>
       <c r="E24">
         <f t="shared" si="2"/>
-        <v>43520624</v>
+        <v>43382212</v>
       </c>
       <c r="F24">
         <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="4"/>
+        <v>[FixedLength(16)]public class Obj540 {}</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="5"/>
+        <v>[InternalReferenceValue(540)] public Obj540[] Obj540s { get; set; }</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>548</v>
+      </c>
+      <c r="C25">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <v>516</v>
-      </c>
-      <c r="C25">
-        <v>288</v>
-      </c>
       <c r="D25">
-        <v>1273744</v>
+        <v>1049652</v>
       </c>
       <c r="E25">
         <f t="shared" si="2"/>
-        <v>43606320</v>
+        <v>43382228</v>
       </c>
       <c r="F25">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="4"/>
+        <v>[FixedLength(80)]public class Obj548 {}</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="5"/>
+        <v>[InternalReferenceValue(548)] public Obj548[] Obj548s { get; set; }</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26">
-        <v>524</v>
+        <v>556</v>
       </c>
       <c r="C26">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>1274032</v>
+        <v>1049732</v>
       </c>
       <c r="E26">
         <f t="shared" si="2"/>
-        <v>43606608</v>
+        <v>43382308</v>
       </c>
       <c r="F26">
         <f t="shared" si="3"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="4"/>
+        <v>[FixedLength(92)]public class Obj556 {}</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="5"/>
+        <v>[InternalReferenceValue(556)] public Obj556[] Obj556s { get; set; }</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27">
-        <v>532</v>
+        <v>564</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27">
-        <v>1274896</v>
+        <v>1049916</v>
       </c>
       <c r="E27">
         <f t="shared" si="2"/>
-        <v>43607472</v>
+        <v>43382492</v>
       </c>
       <c r="F27">
         <f t="shared" si="3"/>
-        <v>220</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>540</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28">
-        <v>1275116</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="2"/>
-        <v>43607692</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <v>548</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29">
-        <v>1275132</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="2"/>
-        <v>43607708</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="3"/>
-        <v>1728</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30">
-        <v>564</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30">
-        <v>1276860</v>
-      </c>
-      <c r="E30">
-        <f t="shared" si="2"/>
-        <v>43609436</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="3"/>
-        <v>-1276860</v>
+        <v>-1049916</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="4"/>
+        <v>[FixedLength(-1049916)]public class Obj564 {}</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="5"/>
+        <v>[InternalReferenceValue(564)] public Obj564[] Obj564s { get; set; }</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I28" t="str">
+        <f t="shared" si="4"/>
+        <v>[FixedLength()]public class Obj {}</v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="5"/>
+        <v>[InternalReferenceValue()] public Obj[] Objs { get; set; }</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I29" t="str">
+        <f t="shared" si="4"/>
+        <v>[FixedLength()]public class Obj {}</v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="5"/>
+        <v>[InternalReferenceValue()] public Obj[] Objs { get; set; }</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I30" t="str">
+        <f t="shared" si="4"/>
+        <v>[FixedLength()]public class Obj {}</v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" si="5"/>
+        <v>[InternalReferenceValue()] public Obj[] Objs { get; set; }</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AD3F75-2402-4656-A232-23962ACADB26}">
+  <dimension ref="B1:L42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="82" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>36</v>
+      </c>
+      <c r="D2">
+        <v>572</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E3" si="0">(D3-D2)/C2</f>
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" t="str">
+        <f>"[FixedLength(" &amp; E2 &amp; ")]public class Obj" &amp; B2 &amp; " {}"</f>
+        <v>[FixedLength(20)]public class Obj12 {}</v>
+      </c>
+      <c r="L2" t="str">
+        <f>"[InternalReferenceValue(" &amp; B2 &amp; ")] public Obj" &amp; B2 &amp; "[] Obj" &amp; B2 &amp; "s { get; set; }"</f>
+        <v>[InternalReferenceValue(12)] public Obj12[] Obj12s { get; set; }</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1292</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>610532</v>
+      </c>
+      <c r="F3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H30" si="1">"[FixedLength(" &amp; E3 &amp; ")]public class Obj" &amp; B3 &amp; " {}"</f>
+        <v>[FixedLength(610532)]public class Obj20 {}</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L31" si="2">"[InternalReferenceValue(" &amp; B3 &amp; ")] public Obj" &amp; B3 &amp; "[] Obj" &amp; B3 &amp; "s { get; set; }"</f>
+        <v>[InternalReferenceValue(20)] public Obj20[] Obj20s { get; set; }</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>44</v>
+      </c>
+      <c r="C4">
+        <v>5427</v>
+      </c>
+      <c r="D4">
+        <v>611824</v>
+      </c>
+      <c r="E4">
+        <f>(D5-D4)/C4</f>
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(8)]public class Obj44 {}</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(44)] public Obj44[] Obj44s { get; set; }</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>76</v>
+      </c>
+      <c r="C5">
+        <v>23580</v>
+      </c>
+      <c r="D5">
+        <v>655240</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E30" si="3">(D6-D5)/C5</f>
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(8)]public class Obj76 {}</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(76)] public Obj76[] Obj76s { get; set; }</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>84</v>
+      </c>
+      <c r="C6">
+        <v>880</v>
+      </c>
+      <c r="D6">
+        <v>843880</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(1)]public class Obj84 {}</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(84)] public Obj84[] Obj84s { get; set; }</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>92</v>
+      </c>
+      <c r="C7">
+        <v>125</v>
+      </c>
+      <c r="D7">
+        <v>844760</v>
+      </c>
+      <c r="E7">
+        <v>36</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(36)]public class Obj92 {}</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(92)] public Obj92[] Obj92s { get; set; }</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>857696</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(24)]public class Obj100 {}</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(100)] public Obj100[] Obj100s { get; set; }</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>148</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>857720</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(36)]public class Obj148 {}</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(148)] public Obj148[] Obj148s { get; set; }</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>156</v>
+      </c>
+      <c r="C10">
+        <v>55</v>
+      </c>
+      <c r="D10">
+        <v>857756</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>612.29090909090905</v>
+      </c>
+      <c r="F10" t="s">
+        <v>88</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(612.290909090909)]public class Obj156 {}</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(156)] public Obj156[] Obj156s { get; set; }</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>164</v>
+      </c>
+      <c r="C11">
+        <v>93</v>
+      </c>
+      <c r="D11">
+        <v>891432</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>34.322580645161288</v>
+      </c>
+      <c r="F11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(34.3225806451613)]public class Obj164 {}</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(164)] public Obj164[] Obj164s { get; set; }</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>172</v>
+      </c>
+      <c r="C12">
+        <v>32</v>
+      </c>
+      <c r="D12">
+        <v>894624</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(2)]public class Obj172 {}</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(172)] public Obj172[] Obj172s { get; set; }</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>212</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>894688</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(100)]public class Obj212 {}</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(212)] public Obj212[] Obj212s { get; set; }</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>220</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>895088</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(72)]public class Obj220 {}</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(220)] public Obj220[] Obj220s { get; set; }</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>244</v>
+      </c>
+      <c r="C15">
+        <v>40</v>
+      </c>
+      <c r="D15">
+        <v>895232</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(16)]public class Obj244 {}</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(244)] public Obj244[] Obj244s { get; set; }</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>252</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>895872</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(20)]public class Obj252 {}</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(252)] public Obj252[] Obj252s { get; set; }</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>260</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>895892</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>104</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(104)]public class Obj260 {}</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(260)] public Obj260[] Obj260s { get; set; }</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>312</v>
+      </c>
+      <c r="C18">
+        <v>19</v>
+      </c>
+      <c r="D18">
+        <v>896204</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>11916.421052631578</v>
+      </c>
+      <c r="F18" t="s">
+        <v>111</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(11916.4210526316)]public class Obj312 {}</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(312)] public Obj312[] Obj312s { get; set; }</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>320</v>
+      </c>
+      <c r="C19">
+        <v>62</v>
+      </c>
+      <c r="D19">
+        <v>1122616</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="3"/>
+        <v>88</v>
+      </c>
+      <c r="F19" t="s">
+        <v>110</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(88)]public class Obj320 {}</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(320)] public Obj320[] Obj320s { get; set; }</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>328</v>
+      </c>
+      <c r="C20">
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>1128072</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="3"/>
+        <v>69.777777777777771</v>
+      </c>
+      <c r="F20" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(69.7777777777778)]public class Obj328 {}</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(328)] public Obj328[] Obj328s { get; set; }</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>336</v>
+      </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <v>1128700</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>68.888888888888886</v>
+      </c>
+      <c r="F21" t="s">
+        <v>101</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(68.8888888888889)]public class Obj336 {}</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(336)] public Obj336[] Obj336s { get; set; }</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>344</v>
+      </c>
+      <c r="C22">
+        <v>34</v>
+      </c>
+      <c r="D22">
+        <v>1129320</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="F22" t="s">
+        <v>104</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(20)]public class Obj344 {}</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(344)] public Obj344[] Obj344s { get; set; }</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>464</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1130000</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="3"/>
+        <v>58048</v>
+      </c>
+      <c r="F23" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(58048)]public class Obj464 {}</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(464)] public Obj464[] Obj464s { get; set; }</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>480</v>
+      </c>
+      <c r="C24">
+        <v>85696</v>
+      </c>
+      <c r="D24">
+        <v>1188048</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>91</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(1)]public class Obj480 {}</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(480)] public Obj480[] Obj480s { get; set; }</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>516</v>
+      </c>
+      <c r="C25">
+        <v>288</v>
+      </c>
+      <c r="D25">
+        <v>1273744</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>91</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(1)]public class Obj516 {}</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(516)] public Obj516[] Obj516s { get; set; }</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>524</v>
+      </c>
+      <c r="C26">
+        <v>27</v>
+      </c>
+      <c r="D26">
+        <v>1274032</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="F26" t="s">
+        <v>105</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(32)]public class Obj524 {}</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(524)] public Obj524[] Obj524s { get; set; }</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>532</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1274896</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="3"/>
+        <v>220</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(220)]public class Obj532 {}</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(532)] public Obj532[] Obj532s { get; set; }</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>540</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1275116</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(16)]public class Obj540 {}</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(540)] public Obj540[] Obj540s { get; set; }</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>548</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1275132</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="3"/>
+        <v>1728</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(1728)]public class Obj548 {}</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(548)] public Obj548[] Obj548s { get; set; }</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>564</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1276860</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="3"/>
+        <v>-1276860</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="1"/>
+        <v>[FixedLength(-1276860)]public class Obj564 {}</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue(564)] public Obj564[] Obj564s { get; set; }</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L31" t="str">
+        <f t="shared" si="2"/>
+        <v>[InternalReferenceValue()] public Obj[] Objs { get; set; }</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>108</v>
+      </c>
+      <c r="E34">
+        <v>22095776</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35">
+        <v>22991980</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>114</v>
+      </c>
+      <c r="E36">
+        <f>E35+11444</f>
+        <v>23003424</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>113</v>
+      </c>
+      <c r="E37">
+        <v>23218392</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <f>E37-E34</f>
+        <v>1122616</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41">
+        <v>23003536</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <f>E41-E36</f>
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF2CFD9-87D1-4455-B2C0-23575B5C5C2A}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>